<commit_message>
Correções sugeridas pela banca da defesa
</commit_message>
<xml_diff>
--- a/Chapter 4/Step 4 - Classifying the Types of Code Readability Improvements/1 - Human Open Coding/Python - Open Coding - samples human evaluation.xlsx
+++ b/Chapter 4/Step 4 - Classifying the Types of Code Readability Improvements/1 - Human Open Coding/Python - Open Coding - samples human evaluation.xlsx
@@ -5584,6 +5584,33 @@
                             )]</t>
   </si>
   <si>
+    <t>path_obj = _coerce_str_or_path_to_path(should_be_path)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Improved the performance test readability, added functions to remove some dup codes.     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactor splitter code to enhance readability (DRY principle).   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I introduced a new `_create_label_group` method to the `PyBadger` class to help improve code readability and reduce code duplication.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first conv in the previous implementation is unnecessary since the input channels can be determined when passing parameters.    ## Modification    The first conv is combined into the loops. Thus, the readability and structure are improved..  </t>
+  </si>
+  <si>
+    <t>Shorten long lines and reduce code repetition</t>
+  </si>
+  <si>
+    <t>Minor PR for refactoring a test. I rewrote the test because I was going to add zarr as another test case, then decided OME-Zarr warrants its own operator and won't go here.    I think the refactoring is still helpful in its own right. It makes the difference between the test cases clearer, and makes sure the h5 and n5 tests don't depend on each other (plus it's a bit shorter :smile: ).    The actual test cases covered and how they're implemented could be improved I think. I'm also not sure about the value of the third test using `.Output.meta.ram_usage_per_requested_pixel = 1000000.0` to force writing in tiny blocks. This test takes 0.5s to run, which is a long time for a test case that seems unnecessary to cover to me. But I intentionally purely refactored here to make review easier.    Note: Squash-merge when re-integrating to main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- deduplicate URL building for GPG key in `install_binary()` (**L394**) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was suggested to use a paramterized test to avoid code duplication in tests.   </t>
+  </si>
+  <si>
     <t>Use f-string</t>
   </si>
   <si>
@@ -5801,33 +5828,6 @@
   </si>
   <si>
     <t>Na Remove Unnecessary Unboxing tem esses imports estáticos</t>
-  </si>
-  <si>
-    <t>path_obj = _coerce_str_or_path_to_path(should_be_path)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Improved the performance test readability, added functions to remove some dup codes.     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refactor splitter code to enhance readability (DRY principle).   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">I introduced a new `_create_label_group` method to the `PyBadger` class to help improve code readability and reduce code duplication.    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The first conv in the previous implementation is unnecessary since the input channels can be determined when passing parameters.    ## Modification    The first conv is combined into the loops. Thus, the readability and structure are improved..  </t>
-  </si>
-  <si>
-    <t>Shorten long lines and reduce code repetition</t>
-  </si>
-  <si>
-    <t>Minor PR for refactoring a test. I rewrote the test because I was going to add zarr as another test case, then decided OME-Zarr warrants its own operator and won't go here.    I think the refactoring is still helpful in its own right. It makes the difference between the test cases clearer, and makes sure the h5 and n5 tests don't depend on each other (plus it's a bit shorter :smile: ).    The actual test cases covered and how they're implemented could be improved I think. I'm also not sure about the value of the third test using `.Output.meta.ram_usage_per_requested_pixel = 1000000.0` to force writing in tiny blocks. This test takes 0.5s to run, which is a long time for a test case that seems unnecessary to cover to me. But I intentionally purely refactored here to make review easier.    Note: Squash-merge when re-integrating to main</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- deduplicate URL building for GPG key in `install_binary()` (**L394**) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">It was suggested to use a paramterized test to avoid code duplication in tests.   </t>
   </si>
   <si>
     <t>It removes a lot of unnecessary code</t>
@@ -23441,152 +23441,121 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>603</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1">
-        <v>80.0</v>
+        <v>2.0</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="9">
-        <v>45097.4934375</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>604</v>
+        <v>45649.62881944444</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>806</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>605</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>606</v>
+        <v>1444</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>808</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I1" s="7"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>608</v>
+        <v>181</v>
       </c>
       <c r="B2" s="1">
-        <v>3.0</v>
+        <v>16.0</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="9">
-        <v>44494.69590277778</v>
+        <v>44894.3253125</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>609</v>
+        <v>940</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>610</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>611</v>
+        <v>941</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I2" s="7"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>612</v>
+        <v>141</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="9">
-        <v>44585.831782407404</v>
+        <v>44012.78587962963</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>614</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>615</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>897</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>220</v>
+        <v>898</v>
       </c>
       <c r="B4" s="1">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="9">
-        <v>44771.56841435185</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>616</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>617</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>618</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>45631.797488425924</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>619</v>
+        <v>900</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="9">
-        <v>45315.880740740744</v>
+        <v>44294.66732638889</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>620</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>621</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>622</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>901</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>623</v>
+        <v>902</v>
       </c>
       <c r="B6" s="1">
         <v>1.0</v>
@@ -23595,27 +23564,19 @@
         <v>10</v>
       </c>
       <c r="D6" s="9">
-        <v>45574.34653935185</v>
+        <v>45218.50853009259</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>624</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>625</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>903</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>904</v>
       </c>
       <c r="B7" s="1">
         <v>1.0</v>
@@ -23624,27 +23585,19 @@
         <v>10</v>
       </c>
       <c r="D7" s="9">
-        <v>43990.70699074074</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>627</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>628</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>42922.74744212963</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>905</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>630</v>
+        <v>907</v>
       </c>
       <c r="B8" s="1">
         <v>1.0</v>
@@ -23653,27 +23606,19 @@
         <v>10</v>
       </c>
       <c r="D8" s="9">
-        <v>44860.90751157407</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>631</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>632</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>633</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>43529.518854166665</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>1446</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>634</v>
+        <v>909</v>
       </c>
       <c r="B9" s="1">
         <v>1.0</v>
@@ -23682,398 +23627,333 @@
         <v>10</v>
       </c>
       <c r="D9" s="9">
-        <v>45293.91193287037</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>635</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>637</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>43875.72231481481</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>638</v>
+        <v>911</v>
       </c>
       <c r="B10" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="9">
-        <v>45373.51615740741</v>
+        <v>45414.86662037037</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>640</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>641</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>912</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>642</v>
+        <v>913</v>
       </c>
       <c r="B11" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="9">
-        <v>45288.72530092593</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>643</v>
+        <v>44842.35505787037</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>1448</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>644</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>645</v>
+        <v>915</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I11" s="7"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>646</v>
+        <v>291</v>
       </c>
       <c r="B12" s="1">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="9">
-        <v>43701.67886574074</v>
+        <v>44887.08230324074</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>647</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>648</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>649</v>
+        <v>916</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I12" s="7"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>650</v>
+        <v>220</v>
       </c>
       <c r="B13" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="9">
-        <v>45235.81371527778</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>651</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>653</v>
+        <v>44771.56841435185</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>1449</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I13" s="7"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>205</v>
+        <v>918</v>
       </c>
       <c r="B14" s="1">
-        <v>8.0</v>
+        <v>1.0</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="9">
-        <v>44033.821597222224</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>654</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>655</v>
+        <v>45517.45982638889</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>1450</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I14" s="7"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>656</v>
+        <v>252</v>
       </c>
       <c r="B15" s="1">
-        <v>1.0</v>
+        <v>25.0</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="9">
-        <v>44397.87590277778</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>657</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>658</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>659</v>
+        <v>45065.47840277778</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>1451</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>921</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>922</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I15" s="7"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>660</v>
+        <v>923</v>
       </c>
       <c r="B16" s="1">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="9">
-        <v>45211.19260416667</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>661</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>662</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>663</v>
+        <v>44881.602314814816</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>1452</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I16" s="7"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>664</v>
+        <v>41</v>
       </c>
       <c r="B17" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="9">
-        <v>45288.32709490741</v>
+        <v>45113.35928240741</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>665</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>666</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>667</v>
+        <v>925</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>809</v>
+      </c>
+      <c r="I17" s="7"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>668</v>
+        <v>522</v>
       </c>
       <c r="B18" s="1">
-        <v>17.0</v>
+        <v>5.0</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="9">
-        <v>43977.821180555555</v>
+        <v>45097.657476851855</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>669</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>670</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>671</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>1444</v>
-      </c>
+        <v>926</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="I18" s="7"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>220</v>
+        <v>603</v>
       </c>
       <c r="B19" s="1">
-        <v>7.0</v>
+        <v>80.0</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="9">
-        <v>44771.56841435185</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>672</v>
+        <v>45097.4934375</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>604</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>673</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>674</v>
+        <v>605</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>606</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>607</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>1445</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>675</v>
+        <v>608</v>
       </c>
       <c r="B20" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="9">
-        <v>44144.7896875</v>
+        <v>44494.69590277778</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>676</v>
+        <v>609</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>677</v>
+        <v>610</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>678</v>
+        <v>611</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>607</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>1446</v>
+      <c r="I20" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>577</v>
+        <v>612</v>
       </c>
       <c r="B21" s="1">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="9">
-        <v>44869.548946759256</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>679</v>
+        <v>44585.831782407404</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>613</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>680</v>
+        <v>614</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>681</v>
+        <v>615</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>607</v>
       </c>
+      <c r="I21" s="7" t="s">
+        <v>1453</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>682</v>
+        <v>220</v>
       </c>
       <c r="B22" s="1">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="9">
-        <v>45043.755520833336</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>683</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>684</v>
+        <v>44771.56841435185</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>617</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>685</v>
+        <v>618</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>687</v>
+        <v>619</v>
       </c>
       <c r="B23" s="1">
         <v>1.0</v>
@@ -24082,24 +23962,27 @@
         <v>10</v>
       </c>
       <c r="D23" s="9">
-        <v>45131.71335648148</v>
+        <v>45315.880740740744</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>1447</v>
+        <v>620</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>1448</v>
+        <v>621</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>1449</v>
+        <v>622</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>691</v>
+        <v>623</v>
       </c>
       <c r="B24" s="1">
         <v>1.0</v>
@@ -24108,76 +23991,85 @@
         <v>10</v>
       </c>
       <c r="D24" s="9">
-        <v>43851.85839120371</v>
+        <v>45574.34653935185</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>1450</v>
+        <v>624</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>1451</v>
+        <v>625</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>1452</v>
+        <v>626</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>695</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D25" s="9">
-        <v>45551.75962962963</v>
-      </c>
-      <c r="E25" s="10" t="s">
+        <v>43990.70699074074</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>628</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>607</v>
+      </c>
+      <c r="I25" s="7" t="s">
         <v>1453</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>1454</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>1455</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>630</v>
       </c>
       <c r="B26" s="1">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D26" s="9">
-        <v>44959.82864583333</v>
+        <v>44860.90751157407</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>699</v>
+        <v>631</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>700</v>
+        <v>632</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>701</v>
+        <v>633</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>702</v>
+        <v>634</v>
       </c>
       <c r="B27" s="1">
         <v>1.0</v>
@@ -24186,102 +24078,114 @@
         <v>10</v>
       </c>
       <c r="D27" s="9">
-        <v>44860.8178125</v>
+        <v>45293.91193287037</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>703</v>
+        <v>635</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>704</v>
+        <v>636</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>705</v>
+        <v>637</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>603</v>
+        <v>638</v>
       </c>
       <c r="B28" s="1">
-        <v>80.0</v>
+        <v>1.0</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D28" s="9">
-        <v>45097.4934375</v>
+        <v>45373.51615740741</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>1456</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>1457</v>
+        <v>639</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>640</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>1458</v>
+        <v>641</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>709</v>
+        <v>642</v>
       </c>
       <c r="B29" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="9">
-        <v>44583.30736111111</v>
+        <v>45288.72530092593</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>710</v>
+        <v>643</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>711</v>
+        <v>644</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>712</v>
+        <v>645</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>503</v>
+        <v>646</v>
       </c>
       <c r="B30" s="1">
-        <v>2.0</v>
+        <v>11.0</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D30" s="9">
-        <v>45208.944560185184</v>
+        <v>43701.67886574074</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>713</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>714</v>
+        <v>647</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>648</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>715</v>
+        <v>649</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>197</v>
+        <v>650</v>
       </c>
       <c r="B31" s="1">
         <v>1.0</v>
@@ -24290,50 +24194,56 @@
         <v>10</v>
       </c>
       <c r="D31" s="9">
-        <v>44778.44204861111</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>716</v>
+        <v>45235.81371527778</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>651</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>717</v>
+        <v>652</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>718</v>
+        <v>653</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B32" s="1">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="9">
-        <v>44771.56841435185</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>719</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>1459</v>
+        <v>44033.821597222224</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>654</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>1460</v>
+        <v>655</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>686</v>
+        <v>607</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>722</v>
+        <v>656</v>
       </c>
       <c r="B33" s="1">
         <v>1.0</v>
@@ -24342,125 +24252,143 @@
         <v>10</v>
       </c>
       <c r="D33" s="9">
-        <v>44502.551840277774</v>
+        <v>44397.87590277778</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>723</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>724</v>
+        <v>657</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>658</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>725</v>
+        <v>659</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>726</v>
+        <v>607</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>252</v>
+        <v>660</v>
       </c>
       <c r="B34" s="1">
-        <v>25.0</v>
+        <v>13.0</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D34" s="9">
-        <v>45065.47840277778</v>
+        <v>45211.19260416667</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>1461</v>
+        <v>661</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>1462</v>
+        <v>662</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>1463</v>
+        <v>663</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>726</v>
+        <v>607</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>730</v>
+        <v>664</v>
       </c>
       <c r="B35" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="9">
-        <v>44970.430439814816</v>
+        <v>45288.32709490741</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>731</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>732</v>
+        <v>665</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>666</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>733</v>
+        <v>667</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>726</v>
+        <v>607</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>965</v>
+        <v>668</v>
       </c>
       <c r="B36" s="1">
-        <v>1.0</v>
+        <v>17.0</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="9">
-        <v>44970.73253472222</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>966</v>
+        <v>43977.821180555555</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>669</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>967</v>
+        <v>670</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>671</v>
       </c>
       <c r="H36" s="7" t="s">
-        <v>726</v>
+        <v>607</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>1453</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>522</v>
+        <v>220</v>
       </c>
       <c r="B37" s="1">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="9">
-        <v>45097.657476851855</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>734</v>
+        <v>44771.56841435185</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>672</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>735</v>
+        <v>673</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>736</v>
+        <v>674</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>726</v>
+        <v>607</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>1454</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>737</v>
+        <v>675</v>
       </c>
       <c r="B38" s="1">
         <v>1.0</v>
@@ -24469,51 +24397,53 @@
         <v>10</v>
       </c>
       <c r="D38" s="9">
-        <v>45566.77664351852</v>
+        <v>44144.7896875</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>738</v>
+        <v>676</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>739</v>
+        <v>677</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>740</v>
+        <v>678</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>726</v>
-      </c>
-      <c r="L38" s="7"/>
+        <v>607</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>1455</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>403</v>
+        <v>577</v>
       </c>
       <c r="B39" s="1">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D39" s="9">
-        <v>45229.917280092595</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>741</v>
+        <v>44869.548946759256</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>679</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>742</v>
+        <v>680</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>743</v>
+        <v>681</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>726</v>
+        <v>607</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>744</v>
+        <v>682</v>
       </c>
       <c r="B40" s="1">
         <v>1.0</v>
@@ -24522,24 +24452,24 @@
         <v>10</v>
       </c>
       <c r="D40" s="9">
-        <v>45565.355</v>
+        <v>45043.755520833336</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>745</v>
+        <v>683</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>1464</v>
+        <v>684</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>747</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>726</v>
+        <v>685</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>752</v>
+        <v>687</v>
       </c>
       <c r="B41" s="1">
         <v>1.0</v>
@@ -24548,24 +24478,24 @@
         <v>10</v>
       </c>
       <c r="D41" s="9">
-        <v>44167.713692129626</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>1465</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>1466</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>1467</v>
+        <v>45131.71335648148</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>1456</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>1458</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>726</v>
+        <v>686</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>756</v>
+        <v>691</v>
       </c>
       <c r="B42" s="1">
         <v>1.0</v>
@@ -24574,128 +24504,128 @@
         <v>10</v>
       </c>
       <c r="D42" s="9">
-        <v>43766.635729166665</v>
+        <v>43851.85839120371</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>757</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>758</v>
+        <v>1459</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>1460</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>759</v>
+        <v>1461</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>760</v>
+        <v>686</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
-        <v>314</v>
+        <v>695</v>
       </c>
       <c r="B43" s="1">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="9">
-        <v>44872.522824074076</v>
+        <v>45551.75962962963</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>761</v>
+        <v>1462</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>762</v>
+        <v>1463</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>763</v>
+        <v>1464</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>760</v>
+        <v>686</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>767</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D44" s="9">
-        <v>44113.43907407407</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>768</v>
+        <v>44959.82864583333</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>699</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>769</v>
+        <v>700</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>770</v>
+        <v>701</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>760</v>
+        <v>686</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>15</v>
+        <v>702</v>
       </c>
       <c r="B45" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D45" s="9">
-        <v>45649.62881944444</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>764</v>
+        <v>44860.8178125</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>703</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>765</v>
+        <v>704</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>766</v>
+        <v>705</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>760</v>
+        <v>686</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="s">
-        <v>771</v>
+        <v>603</v>
       </c>
       <c r="B46" s="1">
-        <v>1.0</v>
+        <v>80.0</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="9">
-        <v>44417.92454861111</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>772</v>
+        <v>45097.4934375</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>1465</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>773</v>
+        <v>1466</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>774</v>
+        <v>1467</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>760</v>
+        <v>686</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
-        <v>775</v>
+        <v>709</v>
       </c>
       <c r="B47" s="1">
         <v>1.0</v>
@@ -24704,50 +24634,50 @@
         <v>10</v>
       </c>
       <c r="D47" s="9">
-        <v>45527.665601851855</v>
+        <v>44583.30736111111</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>1468</v>
+        <v>710</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>777</v>
+        <v>711</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>778</v>
+        <v>712</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>760</v>
+        <v>686</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>279</v>
+        <v>503</v>
       </c>
       <c r="B48" s="1">
         <v>2.0</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="D48" s="9">
-        <v>44412.98415509259</v>
+        <v>45208.944560185184</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>958</v>
+        <v>713</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>1469</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>1470</v>
-      </c>
-      <c r="H48" s="10" t="s">
-        <v>787</v>
+        <v>714</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>783</v>
+        <v>197</v>
       </c>
       <c r="B49" s="1">
         <v>1.0</v>
@@ -24756,140 +24686,128 @@
         <v>10</v>
       </c>
       <c r="D49" s="9">
-        <v>45609.0327662037</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>784</v>
+        <v>44778.44204861111</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>716</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>785</v>
+        <v>717</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>786</v>
+        <v>718</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>787</v>
+        <v>686</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="s">
-        <v>603</v>
+        <v>220</v>
       </c>
       <c r="B50" s="1">
-        <v>80.0</v>
+        <v>7.0</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D50" s="9">
-        <v>45097.4934375</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>788</v>
+        <v>44771.56841435185</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>719</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>789</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>790</v>
+        <v>1468</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>1469</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>787</v>
-      </c>
-      <c r="I50" s="7" t="s">
-        <v>1471</v>
+        <v>686</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
-        <v>603</v>
+        <v>722</v>
       </c>
       <c r="B51" s="1">
-        <v>80.0</v>
+        <v>1.0</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D51" s="9">
-        <v>45097.4934375</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>604</v>
+        <v>44502.551840277774</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>723</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>791</v>
+        <v>724</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>792</v>
+        <v>725</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>787</v>
-      </c>
-      <c r="I51" s="7" t="s">
-        <v>1471</v>
+        <v>726</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="s">
-        <v>687</v>
+        <v>252</v>
       </c>
       <c r="B52" s="1">
-        <v>1.0</v>
+        <v>25.0</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D52" s="9">
-        <v>45131.71335648148</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>793</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>794</v>
+        <v>45065.47840277778</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>1470</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>1471</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>795</v>
+        <v>1472</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>787</v>
-      </c>
-      <c r="I52" s="7" t="s">
-        <v>1471</v>
+        <v>726</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
-        <v>314</v>
+        <v>730</v>
       </c>
       <c r="B53" s="1">
-        <v>9.0</v>
+        <v>2.0</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D53" s="9">
-        <v>44872.522824074076</v>
+        <v>44970.430439814816</v>
       </c>
       <c r="E53" s="10" t="s">
-        <v>796</v>
+        <v>731</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>797</v>
+        <v>732</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>798</v>
+        <v>733</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>787</v>
-      </c>
-      <c r="I53" s="7" t="s">
-        <v>1471</v>
+        <v>726</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="s">
-        <v>1374</v>
+        <v>965</v>
       </c>
       <c r="B54" s="1">
         <v>1.0</v>
@@ -24898,102 +24816,100 @@
         <v>10</v>
       </c>
       <c r="D54" s="9">
-        <v>43994.675150462965</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>1375</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>1376</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>1377</v>
+        <v>44970.73253472222</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>967</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>239</v>
+        <v>726</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
-        <v>799</v>
+        <v>522</v>
       </c>
       <c r="B55" s="1">
-        <v>11.0</v>
+        <v>5.0</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D55" s="9">
-        <v>43974.516226851854</v>
+        <v>45097.657476851855</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>800</v>
-      </c>
-      <c r="F55" s="10" t="s">
-        <v>801</v>
+        <v>734</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>735</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>802</v>
+        <v>736</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>239</v>
+        <v>726</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="s">
-        <v>275</v>
+        <v>737</v>
       </c>
       <c r="B56" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="9">
-        <v>45591.861863425926</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>1472</v>
+        <v>45566.77664351852</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>738</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>1473</v>
+        <v>739</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>1474</v>
+        <v>740</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>239</v>
-      </c>
+        <v>726</v>
+      </c>
+      <c r="L56" s="7"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
-        <v>252</v>
+        <v>403</v>
       </c>
       <c r="B57" s="1">
-        <v>25.0</v>
+        <v>1.0</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D57" s="9">
-        <v>45065.47840277778</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>1475</v>
+        <v>45229.917280092595</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>741</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>984</v>
+        <v>742</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>985</v>
-      </c>
-      <c r="H57" s="10" t="s">
-        <v>239</v>
+        <v>743</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>726</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="s">
-        <v>235</v>
+        <v>744</v>
       </c>
       <c r="B58" s="1">
         <v>1.0</v>
@@ -25002,24 +24918,24 @@
         <v>10</v>
       </c>
       <c r="D58" s="9">
-        <v>45366.641597222224</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>237</v>
+        <v>45565.355</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>1473</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>1476</v>
+        <v>747</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>239</v>
+        <v>726</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
-        <v>813</v>
+        <v>752</v>
       </c>
       <c r="B59" s="1">
         <v>1.0</v>
@@ -25028,623 +24944,1103 @@
         <v>10</v>
       </c>
       <c r="D59" s="9">
-        <v>44907.60824074074</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>1477</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>1478</v>
-      </c>
-      <c r="G59" s="7" t="s">
-        <v>1479</v>
+        <v>44167.713692129626</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>1474</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>1476</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>239</v>
+        <v>726</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="s">
-        <v>864</v>
+        <v>756</v>
       </c>
       <c r="B60" s="1">
         <v>1.0</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="D60" s="9">
-        <v>43867.87763888889</v>
+        <v>43766.635729166665</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>865</v>
+        <v>757</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>866</v>
+        <v>758</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>867</v>
+        <v>759</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>239</v>
+        <v>760</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
-        <v>868</v>
+        <v>314</v>
       </c>
       <c r="B61" s="1">
-        <v>4.0</v>
+        <v>9.0</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D61" s="9">
-        <v>44293.83957175926</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>869</v>
+        <v>44872.522824074076</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>761</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>870</v>
+        <v>762</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>871</v>
+        <v>763</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>239</v>
+        <v>760</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="s">
-        <v>363</v>
+        <v>767</v>
       </c>
       <c r="B62" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D62" s="9">
-        <v>44813.54857638889</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>364</v>
+        <v>44113.43907407407</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>768</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>1480</v>
+        <v>769</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>366</v>
+        <v>770</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>367</v>
+        <v>760</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
-        <v>358</v>
+        <v>15</v>
       </c>
       <c r="B63" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D63" s="9">
-        <v>44066.038402777776</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>817</v>
+        <v>45649.62881944444</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>764</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>818</v>
+        <v>765</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>819</v>
+        <v>766</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>367</v>
+        <v>760</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="s">
-        <v>503</v>
+        <v>771</v>
       </c>
       <c r="B64" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D64" s="9">
-        <v>45208.944560185184</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>820</v>
+        <v>44417.92454861111</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>772</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>821</v>
+        <v>773</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>822</v>
+        <v>774</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>367</v>
+        <v>760</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
-        <v>252</v>
+        <v>775</v>
       </c>
       <c r="B65" s="1">
-        <v>25.0</v>
+        <v>1.0</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D65" s="9">
-        <v>45065.47840277778</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>823</v>
+        <v>45527.665601851855</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>1477</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>824</v>
+        <v>777</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>825</v>
+        <v>778</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>367</v>
+        <v>760</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="s">
-        <v>522</v>
+        <v>279</v>
       </c>
       <c r="B66" s="1">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="D66" s="9">
-        <v>45097.657476851855</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>826</v>
+        <v>44412.98415509259</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>958</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>827</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>828</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>367</v>
+        <v>1478</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>1479</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="s">
-        <v>15</v>
+        <v>783</v>
       </c>
       <c r="B67" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D67" s="9">
-        <v>45649.62881944444</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>748</v>
-      </c>
-      <c r="F67" s="7" t="s">
-        <v>749</v>
+        <v>45609.0327662037</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>785</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>750</v>
-      </c>
-      <c r="H67" s="10" t="s">
-        <v>751</v>
+        <v>786</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="s">
-        <v>314</v>
+        <v>603</v>
       </c>
       <c r="B68" s="1">
-        <v>9.0</v>
+        <v>80.0</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D68" s="9">
-        <v>44872.522824074076</v>
-      </c>
-      <c r="E68" s="10" t="s">
-        <v>829</v>
+        <v>45097.4934375</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>788</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>830</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>831</v>
+        <v>789</v>
+      </c>
+      <c r="G68" s="10" t="s">
+        <v>790</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>751</v>
+        <v>787</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>1480</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="s">
-        <v>302</v>
+        <v>603</v>
       </c>
       <c r="B69" s="1">
-        <v>2.0</v>
+        <v>80.0</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D69" s="9">
-        <v>45072.81421296296</v>
+        <v>45097.4934375</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>832</v>
+        <v>604</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>833</v>
+        <v>791</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="H69" s="10" t="s">
-        <v>751</v>
+        <v>792</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>1480</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="s">
-        <v>835</v>
+        <v>687</v>
       </c>
       <c r="B70" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D70" s="9">
-        <v>45455.74741898148</v>
+        <v>45131.71335648148</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>1405</v>
+        <v>793</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>1481</v>
+        <v>794</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>1482</v>
-      </c>
-      <c r="H70" s="10" t="s">
-        <v>751</v>
+        <v>795</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>787</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>1480</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="s">
-        <v>839</v>
+        <v>314</v>
       </c>
       <c r="B71" s="1">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D71" s="9">
-        <v>45636.403715277775</v>
+        <v>44872.522824074076</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>840</v>
+        <v>796</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>1483</v>
+        <v>797</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>1484</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>843</v>
+        <v>798</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>787</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>1485</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="s">
-        <v>844</v>
+        <v>1374</v>
       </c>
       <c r="B72" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D72" s="9">
-        <v>45007.44865740741</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>845</v>
+        <v>43994.675150462965</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>1375</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>846</v>
+        <v>1376</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>847</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>843</v>
+        <v>1377</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="s">
-        <v>848</v>
+        <v>799</v>
       </c>
       <c r="B73" s="1">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D73" s="9">
-        <v>43777.932534722226</v>
+        <v>43974.516226851854</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>849</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>850</v>
+        <v>800</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>801</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>851</v>
-      </c>
-      <c r="H73" s="10" t="s">
-        <v>843</v>
+        <v>802</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="s">
-        <v>33</v>
+        <v>275</v>
       </c>
       <c r="B74" s="1">
-        <v>11.0</v>
+        <v>2.0</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D74" s="9">
-        <v>45063.459756944445</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>529</v>
+        <v>45591.861863425926</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>1481</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>530</v>
+        <v>1482</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>531</v>
+        <v>1483</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>532</v>
+        <v>239</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="s">
-        <v>533</v>
+        <v>252</v>
       </c>
       <c r="B75" s="1">
-        <v>1.0</v>
+        <v>25.0</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D75" s="9">
-        <v>44184.641493055555</v>
-      </c>
-      <c r="E75" s="10" t="s">
-        <v>534</v>
+        <v>45065.47840277778</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>1484</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>535</v>
+        <v>984</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="H75" s="7" t="s">
-        <v>532</v>
+        <v>985</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="s">
-        <v>608</v>
+        <v>235</v>
       </c>
       <c r="B76" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D76" s="9">
-        <v>44494.69590277778</v>
-      </c>
-      <c r="E76" s="10" t="s">
-        <v>856</v>
+        <v>45366.641597222224</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>857</v>
+        <v>237</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>858</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>532</v>
+        <v>1485</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="s">
-        <v>859</v>
+        <v>813</v>
       </c>
       <c r="B77" s="1">
-        <v>24.0</v>
+        <v>1.0</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D77" s="9">
-        <v>44887.85392361111</v>
+        <v>44907.60824074074</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>860</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>861</v>
-      </c>
-      <c r="G77" s="10" t="s">
-        <v>862</v>
+        <v>1486</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>1487</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>1488</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>863</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="B78" s="1">
         <v>1.0</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>10</v>
+        <v>280</v>
       </c>
       <c r="D78" s="9">
-        <v>45656.0190625</v>
+        <v>43867.87763888889</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>873</v>
-      </c>
-      <c r="F78" s="10" t="s">
-        <v>874</v>
-      </c>
-      <c r="G78" s="10" t="s">
-        <v>875</v>
+        <v>865</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>867</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>876</v>
+        <v>239</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="s">
-        <v>877</v>
+        <v>868</v>
       </c>
       <c r="B79" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D79" s="9">
-        <v>45628.31726851852</v>
+        <v>44293.83957175926</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>878</v>
+        <v>869</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>879</v>
-      </c>
-      <c r="G79" s="10" t="s">
-        <v>880</v>
+        <v>870</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>871</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>876</v>
+        <v>239</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="s">
-        <v>608</v>
+        <v>363</v>
       </c>
       <c r="B80" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D80" s="9">
-        <v>44494.69590277778</v>
+        <v>44813.54857638889</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>881</v>
+        <v>364</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>882</v>
-      </c>
-      <c r="G80" s="10" t="s">
-        <v>883</v>
-      </c>
-      <c r="H80" s="17" t="s">
-        <v>884</v>
-      </c>
-      <c r="I80" s="7"/>
+        <v>1489</v>
+      </c>
+      <c r="G80" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81" s="9">
+        <v>44066.038402777776</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>819</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="B82" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" s="9">
+        <v>45208.944560185184</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>820</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B83" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="9">
+        <v>45065.47840277778</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>823</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>825</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="B84" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" s="9">
+        <v>45097.657476851855</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>826</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B85" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85" s="9">
+        <v>45649.62881944444</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B86" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" s="9">
+        <v>44872.522824074076</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>831</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B87" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" s="9">
+        <v>45072.81421296296</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>832</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="B88" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88" s="9">
+        <v>45455.74741898148</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>1405</v>
+      </c>
+      <c r="F88" s="10" t="s">
+        <v>1490</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>1491</v>
+      </c>
+      <c r="H88" s="10" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="B89" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89" s="9">
+        <v>45636.403715277775</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>1492</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>1493</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>843</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="B90" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="9">
+        <v>45007.44865740741</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>845</v>
+      </c>
+      <c r="F90" s="10" t="s">
+        <v>846</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="B91" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91" s="9">
+        <v>43777.932534722226</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>851</v>
+      </c>
+      <c r="H91" s="10" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92" s="9">
+        <v>45063.459756944445</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="H92" s="7" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="B93" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D93" s="9">
+        <v>44184.641493055555</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>534</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B94" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94" s="9">
+        <v>44494.69590277778</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>856</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>857</v>
+      </c>
+      <c r="G94" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="H94" s="7" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="B95" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95" s="9">
+        <v>44887.85392361111</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>860</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>861</v>
+      </c>
+      <c r="G95" s="10" t="s">
+        <v>862</v>
+      </c>
+      <c r="H95" s="7" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D96" s="9">
+        <v>45656.0190625</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="F96" s="10" t="s">
+        <v>874</v>
+      </c>
+      <c r="G96" s="10" t="s">
+        <v>875</v>
+      </c>
+      <c r="H96" s="7" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" s="9">
+        <v>45628.31726851852</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>878</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>879</v>
+      </c>
+      <c r="G97" s="10" t="s">
+        <v>880</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="B98" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D98" s="9">
+        <v>44494.69590277778</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>881</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>882</v>
+      </c>
+      <c r="G98" s="10" t="s">
+        <v>883</v>
+      </c>
+      <c r="H98" s="17" t="s">
+        <v>884</v>
+      </c>
+      <c r="I98" s="7"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="s">
         <v>889</v>
       </c>
-      <c r="B81" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D81" s="9">
+      <c r="B99" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="9">
         <v>44363.302349537036</v>
       </c>
-      <c r="E81" s="7" t="s">
+      <c r="E99" s="7" t="s">
         <v>890</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F99" s="7" t="s">
         <v>891</v>
       </c>
-      <c r="G81" s="7" t="s">
+      <c r="G99" s="7" t="s">
         <v>892</v>
       </c>
-      <c r="H81" s="7" t="s">
+      <c r="H99" s="7" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="137">
-      <c r="I137" s="7"/>
-    </row>
-    <row r="138">
-      <c r="I138" s="7"/>
-    </row>
-    <row r="139">
-      <c r="I139" s="7"/>
-    </row>
-    <row r="140">
-      <c r="I140" s="7"/>
-    </row>
-    <row r="141">
-      <c r="I141" s="7"/>
-    </row>
-    <row r="142">
-      <c r="I142" s="7"/>
-    </row>
-    <row r="143">
-      <c r="I143" s="7"/>
-    </row>
-    <row r="144">
-      <c r="I144" s="7"/>
-    </row>
-    <row r="146">
-      <c r="I146" s="7"/>
+    <row r="155">
+      <c r="I155" s="7"/>
+    </row>
+    <row r="156">
+      <c r="I156" s="7"/>
+    </row>
+    <row r="157">
+      <c r="I157" s="7"/>
+    </row>
+    <row r="158">
+      <c r="I158" s="7"/>
+    </row>
+    <row r="159">
+      <c r="I159" s="7"/>
+    </row>
+    <row r="160">
+      <c r="I160" s="7"/>
+    </row>
+    <row r="161">
+      <c r="I161" s="7"/>
+    </row>
+    <row r="162">
+      <c r="I162" s="7"/>
+    </row>
+    <row r="164">
+      <c r="I164" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -25729,8 +26125,26 @@
     <hyperlink r:id="rId79" ref="A79"/>
     <hyperlink r:id="rId80" ref="A80"/>
     <hyperlink r:id="rId81" ref="A81"/>
+    <hyperlink r:id="rId82" ref="A82"/>
+    <hyperlink r:id="rId83" ref="A83"/>
+    <hyperlink r:id="rId84" ref="A84"/>
+    <hyperlink r:id="rId85" ref="A85"/>
+    <hyperlink r:id="rId86" ref="A86"/>
+    <hyperlink r:id="rId87" ref="A87"/>
+    <hyperlink r:id="rId88" ref="A88"/>
+    <hyperlink r:id="rId89" ref="A89"/>
+    <hyperlink r:id="rId90" ref="A90"/>
+    <hyperlink r:id="rId91" ref="A91"/>
+    <hyperlink r:id="rId92" ref="A92"/>
+    <hyperlink r:id="rId93" ref="A93"/>
+    <hyperlink r:id="rId94" ref="A94"/>
+    <hyperlink r:id="rId95" ref="A95"/>
+    <hyperlink r:id="rId96" ref="A96"/>
+    <hyperlink r:id="rId97" ref="A97"/>
+    <hyperlink r:id="rId98" ref="A98"/>
+    <hyperlink r:id="rId99" ref="A99"/>
   </hyperlinks>
-  <drawing r:id="rId82"/>
+  <drawing r:id="rId100"/>
 </worksheet>
 </file>
 
@@ -25752,76 +26166,73 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="9">
-        <v>45649.62881944444</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>806</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>1486</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>808</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>809</v>
+        <v>45113.35928240741</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>927</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>181</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
-        <v>16.0</v>
+        <v>11.0</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="9">
-        <v>44894.3253125</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>940</v>
+        <v>45063.459756944445</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>930</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>941</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>809</v>
+        <v>931</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>141</v>
+        <v>932</v>
       </c>
       <c r="B3" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="9">
-        <v>44012.78587962963</v>
+        <v>44328.03145833333</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>897</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>809</v>
+        <v>933</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>934</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>898</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1">
         <v>6.0</v>
@@ -25830,58 +26241,64 @@
         <v>10</v>
       </c>
       <c r="D4" s="9">
-        <v>45631.797488425924</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>1487</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>809</v>
+        <v>44299.035578703704</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>935</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>936</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>900</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="9">
-        <v>44294.66732638889</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>901</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>809</v>
+        <v>44962.67138888889</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>902</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="9">
-        <v>45218.50853009259</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>903</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>809</v>
+        <v>45384.92670138889</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>939</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>904</v>
+        <v>197</v>
       </c>
       <c r="B7" s="1">
         <v>1.0</v>
@@ -25890,141 +26307,160 @@
         <v>10</v>
       </c>
       <c r="D7" s="9">
-        <v>42922.74744212963</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>905</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>809</v>
+        <v>44778.44204861111</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>907</v>
+        <v>125</v>
       </c>
       <c r="B8" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="9">
-        <v>43529.518854166665</v>
+        <v>44888.91270833334</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>1488</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>809</v>
+        <v>944</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>909</v>
+        <v>946</v>
       </c>
       <c r="B9" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="9">
-        <v>43875.72231481481</v>
+        <v>44298.53172453704</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>1489</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>809</v>
+        <v>1495</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>948</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>911</v>
+        <v>687</v>
       </c>
       <c r="B10" s="1">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="9">
-        <v>45414.86662037037</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>912</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>809</v>
+        <v>45131.71335648148</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>1496</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>950</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>913</v>
+        <v>951</v>
       </c>
       <c r="B11" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="9">
-        <v>44842.35505787037</v>
+        <v>45454.71513888889</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>1490</v>
+        <v>952</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>809</v>
+        <v>1497</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>291</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1">
-        <v>13.0</v>
+        <v>2.0</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="9">
-        <v>44887.08230324074</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>916</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>809</v>
+        <v>45649.62881944444</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>220</v>
+        <v>962</v>
       </c>
       <c r="B13" s="1">
-        <v>7.0</v>
+        <v>2.0</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="9">
-        <v>44771.56841435185</v>
+        <v>45104.14184027778</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>1491</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>809</v>
+        <v>963</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>918</v>
+        <v>968</v>
       </c>
       <c r="B14" s="1">
         <v>1.0</v>
@@ -26033,216 +26469,246 @@
         <v>10</v>
       </c>
       <c r="D14" s="9">
-        <v>45517.45982638889</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>1492</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>809</v>
+        <v>45376.80880787037</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>1498</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>1500</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>252</v>
+        <v>752</v>
       </c>
       <c r="B15" s="1">
-        <v>25.0</v>
+        <v>1.0</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="9">
-        <v>45065.47840277778</v>
+        <v>44167.713692129626</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>1493</v>
+        <v>1501</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>921</v>
+        <v>1502</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>922</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>809</v>
+        <v>1503</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>923</v>
+        <v>668</v>
       </c>
       <c r="B16" s="1">
-        <v>1.0</v>
+        <v>17.0</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="9">
-        <v>44881.602314814816</v>
+        <v>43977.821180555555</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>1494</v>
+        <v>990</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>991</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>809</v>
+        <v>888</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>41</v>
+        <v>216</v>
       </c>
       <c r="B17" s="1">
-        <v>4.0</v>
+        <v>30.0</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="9">
-        <v>45113.35928240741</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>925</v>
+        <v>45054.74172453704</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>993</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>809</v>
+        <v>888</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>522</v>
+        <v>608</v>
       </c>
       <c r="B18" s="1">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="9">
-        <v>45097.657476851855</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>926</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>809</v>
+        <v>44494.69590277778</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>886</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>887</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>888</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>41</v>
+        <v>220</v>
       </c>
       <c r="B19" s="1">
-        <v>4.0</v>
+        <v>7.0</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="9">
-        <v>45113.35928240741</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>927</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>929</v>
+        <v>44771.56841435185</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>975</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>976</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>977</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>978</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>33</v>
+        <v>979</v>
       </c>
       <c r="B20" s="1">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="9">
-        <v>45063.459756944445</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>930</v>
+        <v>45509.659363425926</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>980</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>931</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>929</v>
+        <v>981</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>982</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>932</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>1.0</v>
+        <v>27.0</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D21" s="9">
-        <v>44328.03145833333</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>933</v>
+        <v>44042.71251157407</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>997</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>934</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>929</v>
+        <v>998</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>999</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>982</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>852</v>
       </c>
       <c r="B22" s="1">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="9">
-        <v>44299.035578703704</v>
+        <v>44092.86241898148</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>935</v>
+        <v>986</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>936</v>
+        <v>987</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>988</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>929</v>
+        <v>989</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="9">
-        <v>44962.67138888889</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>937</v>
+        <v>44299.035578703704</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>994</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>938</v>
-      </c>
-      <c r="H23" s="10" t="s">
-        <v>929</v>
+        <v>995</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>996</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>517</v>
       </c>
       <c r="B24" s="1">
         <v>2.0</v>
@@ -26251,445 +26717,15 @@
         <v>10</v>
       </c>
       <c r="D24" s="9">
-        <v>45384.92670138889</v>
+        <v>44465.3719212963</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>939</v>
+        <v>954</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>1504</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="9">
-        <v>44778.44204861111</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>942</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>943</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="9">
-        <v>44888.91270833334</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>944</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>945</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="s">
-        <v>946</v>
-      </c>
-      <c r="B27" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" s="9">
-        <v>44298.53172453704</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>1495</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>948</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>687</v>
-      </c>
-      <c r="B28" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="9">
-        <v>45131.71335648148</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>1496</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>950</v>
-      </c>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="s">
-        <v>951</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="9">
-        <v>45454.71513888889</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>952</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>1497</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="9">
-        <v>45649.62881944444</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>764</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>961</v>
-      </c>
-      <c r="H30" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="s">
-        <v>962</v>
-      </c>
-      <c r="B31" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="9">
-        <v>45104.14184027778</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>964</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="s">
-        <v>968</v>
-      </c>
-      <c r="B32" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="9">
-        <v>45376.80880787037</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>1498</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>1499</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>1500</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="s">
-        <v>752</v>
-      </c>
-      <c r="B33" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="9">
-        <v>44167.713692129626</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>1501</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>1502</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>1503</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="B34" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" s="9">
-        <v>43977.821180555555</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>990</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>991</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B35" s="1">
-        <v>30.0</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="9">
-        <v>45054.74172453704</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>992</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>993</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="B36" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D36" s="9">
-        <v>44494.69590277778</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>885</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>886</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>887</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="B37" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" s="9">
-        <v>44771.56841435185</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>975</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>976</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>977</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>979</v>
-      </c>
-      <c r="B38" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="9">
-        <v>45509.659363425926</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>980</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>981</v>
-      </c>
-      <c r="H38" s="7" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B39" s="1">
-        <v>27.0</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D39" s="9">
-        <v>44042.71251157407</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>997</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>998</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>999</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="B40" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D40" s="9">
-        <v>44092.86241898148</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>986</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>987</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>988</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="1">
-        <v>6.0</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="9">
-        <v>44299.035578703704</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>994</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>995</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="B42" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="9">
-        <v>44465.3719212963</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>954</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>1504</v>
-      </c>
-      <c r="H42" s="10" t="s">
         <v>1505</v>
       </c>
     </row>
@@ -26719,26 +26755,8 @@
     <hyperlink r:id="rId22" ref="A22"/>
     <hyperlink r:id="rId23" ref="A23"/>
     <hyperlink r:id="rId24" ref="A24"/>
-    <hyperlink r:id="rId25" ref="A25"/>
-    <hyperlink r:id="rId26" ref="A26"/>
-    <hyperlink r:id="rId27" ref="A27"/>
-    <hyperlink r:id="rId28" ref="A28"/>
-    <hyperlink r:id="rId29" ref="A29"/>
-    <hyperlink r:id="rId30" ref="A30"/>
-    <hyperlink r:id="rId31" ref="A31"/>
-    <hyperlink r:id="rId32" ref="A32"/>
-    <hyperlink r:id="rId33" ref="A33"/>
-    <hyperlink r:id="rId34" ref="A34"/>
-    <hyperlink r:id="rId35" ref="A35"/>
-    <hyperlink r:id="rId36" ref="A36"/>
-    <hyperlink r:id="rId37" ref="A37"/>
-    <hyperlink r:id="rId38" ref="A38"/>
-    <hyperlink r:id="rId39" ref="A39"/>
-    <hyperlink r:id="rId40" ref="A40"/>
-    <hyperlink r:id="rId41" ref="A41"/>
-    <hyperlink r:id="rId42" ref="A42"/>
   </hyperlinks>
-  <drawing r:id="rId43"/>
+  <drawing r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>